<commit_message>
Support loading rules from local storage
</commit_message>
<xml_diff>
--- a/patient-flags/src/test/resources/org/openmrs/module/drools/patientflags/test_sepsis_rules_table.drl.xlsx
+++ b/patient-flags/src/test/resources/org/openmrs/module/drools/patientflags/test_sepsis_rules_table.drl.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t xml:space="preserve">RuleSet</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Variables</t>
   </si>
   <si>
-    <t xml:space="preserve">org.openmrs.module.drools.calculation.DroolsCalculationService calculationService, String SYSTOLIC_UUID,  java.util.List flaggedPatients</t>
+    <t xml:space="preserve">org.openmrs.module.drools.calculation.DroolsCalculationService service</t>
   </si>
   <si>
     <t xml:space="preserve">agenda-group</t>
@@ -76,16 +76,16 @@
     <t xml:space="preserve">age &gt; $param</t>
   </si>
   <si>
-    <t xml:space="preserve">calculationService.checkObs($patient, "CIEL:5088", Operator.GTE, daysAgo(1)).matches(Operator.GT, $1) || calculationService.checkObs($patient, "CIEL:5088", Operator.GTE, daysAgo(1)).matches(Operator.LT, $2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculationService.checkObs($patient, "CIEL:5087", Operator.GTE, daysAgo(1)).matches(Operator.GT, $param)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculationService.checkObs($patient, "CIEL:5242", Operator.GTE, daysAgo(1)).matches(Operator.GT, $param)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">calculationService.checkObs($patient, "CIEL:5085", Operator.GTE, daysAgo(1)).matches(Operator.LT, $param)</t>
+    <t xml:space="preserve">service.checkObs($patient, "CIEL:5088", Operator.GTE, daysAgo(1)).matches(Operator.GT, $1) || service.checkObs($patient, "CIEL:5088", Operator.GTE, daysAgo(1)).matches(Operator.LT, $2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service.checkObs($patient, "CIEL:5087", Operator.GTE, daysAgo(1)).matches(Operator.GT, $param)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service.checkObs($patient, "CIEL:5242", Operator.GTE, daysAgo(1)).matches(Operator.GT, $param)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service.checkObs($patient, "CIEL:5085", Operator.GTE, daysAgo(1)).matches(Operator.LT, $param)</t>
   </si>
   <si>
     <t xml:space="preserve">not FlaggedPatient(patientId == $patient.getId())</t>
@@ -94,18 +94,12 @@
     <t xml:space="preserve">$flag: FlaggedPatient(patientId == $patient.getId(), message == $param)</t>
   </si>
   <si>
-    <t xml:space="preserve">$flag: FlaggedPatient()</t>
-  </si>
-  <si>
     <t xml:space="preserve">insert(new FlaggedPatient($patient.getId(), $param));</t>
   </si>
   <si>
     <t xml:space="preserve">modify($flag){ setMessage($param) }</t>
   </si>
   <si>
-    <t xml:space="preserve">flaggedPatients.add($flag);</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rule Name</t>
   </si>
   <si>
@@ -127,10 +121,7 @@
     <t xml:space="preserve">No Existing Sepsis Flag</t>
   </si>
   <si>
-    <t xml:space="preserve">Has Sepsis Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not in FlaggedPatient List</t>
+    <t xml:space="preserve">Has Sepsis Flag With Message</t>
   </si>
   <si>
     <t xml:space="preserve">Flag Patient</t>
@@ -139,10 +130,7 @@
     <t xml:space="preserve">Set Sepsis Severe </t>
   </si>
   <si>
-    <t xml:space="preserve">Export Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Sepsis Warning 1</t>
+    <t xml:space="preserve">Sepsis Warning 1</t>
   </si>
   <si>
     <t xml:space="preserve">All 3 Symptoms</t>
@@ -154,37 +142,31 @@
     <t xml:space="preserve">"Sepsis Warning"</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Sepsis Warning 2</t>
+    <t xml:space="preserve">Sepsis Warning 2</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature &amp; Pulse</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Sepsis Warning 3</t>
+    <t xml:space="preserve">Sepsis Warning 3</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature &amp; Respiratory Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Sepsis Warning 4</t>
+    <t xml:space="preserve">Sepsis Warning 4</t>
   </si>
   <si>
     <t xml:space="preserve">Pulse &amp; Respiratory Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Sepsis  Severe</t>
+    <t xml:space="preserve">Sepsis  Severe</t>
   </si>
   <si>
     <t xml:space="preserve">Sepsis Warning &amp; Systolic Pressure</t>
   </si>
   <si>
     <t xml:space="preserve">"Severe Sepsis"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Export Flag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">execute</t>
   </si>
 </sst>
 </file>
@@ -276,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -327,10 +309,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -522,10 +500,10 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -536,9 +514,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="72.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="2" width="29.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="29.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="3" width="34.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="34.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="23.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="23.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -553,7 +532,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -567,7 +546,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -581,7 +560,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="K3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -595,7 +574,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="K4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
@@ -610,7 +589,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="K5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
@@ -625,7 +604,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="K6" s="4"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="9"/>
@@ -635,7 +614,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="K7" s="4"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
@@ -649,7 +628,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="K8" s="4"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
@@ -679,16 +658,10 @@
       <c r="I9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -702,7 +675,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="K10" s="4"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4"/>
@@ -728,70 +701,58 @@
       <c r="I11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="H12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="J12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="6" t="n">
         <v>18</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E13" s="6" t="n">
         <v>90</v>
@@ -805,23 +766,22 @@
         <v>1</v>
       </c>
       <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="4" t="s">
-        <v>43</v>
+      <c r="J13" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>18</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E14" s="6" t="n">
         <v>90</v>
@@ -833,23 +793,22 @@
         <v>1</v>
       </c>
       <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="4" t="s">
-        <v>43</v>
+      <c r="J14" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C15" s="6" t="n">
         <v>18</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="n">
@@ -861,17 +820,16 @@
         <v>1</v>
       </c>
       <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="4" t="s">
-        <v>43</v>
+      <c r="J15" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>18</v>
@@ -889,17 +847,16 @@
         <v>1</v>
       </c>
       <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="12" t="s">
-        <v>43</v>
+      <c r="J16" s="12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>18</v>
@@ -908,25 +865,13 @@
         <v>90</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="L17" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J18" s="13" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
+        <v>39</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C10:G10"/>

</xml_diff>

<commit_message>
Drop usage of FlaggedPatient and remove unused providers
</commit_message>
<xml_diff>
--- a/patient-flags/src/test/resources/org/openmrs/module/drools/patientflags/test_sepsis_rules_table.drl.xlsx
+++ b/patient-flags/src/test/resources/org/openmrs/module/drools/patientflags/test_sepsis_rules_table.drl.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Import</t>
   </si>
   <si>
-    <t xml:space="preserve">org.openmrs.Patient,org.openmrs.module.drools.patientflags.FlaggedPatient,org.openmrs.module.drools.calculation.Operator, static org.openmrs.module.drools.utils.DroolsDateUtils.daysAgo</t>
+    <t xml:space="preserve">org.openmrs.Patient,org.openmrs.module.patientflags.PatientFlag,org.openmrs.module.drools.calculation.Operator, static org.openmrs.module.drools.utils.DroolsDateUtils.daysAgo</t>
   </si>
   <si>
     <t xml:space="preserve">Variables</t>
@@ -88,13 +88,13 @@
     <t xml:space="preserve">service.checkObs($patient, "CIEL:5085", Operator.GTE, daysAgo(1)).matches(Operator.LT, $param)</t>
   </si>
   <si>
-    <t xml:space="preserve">not FlaggedPatient(patientId == $patient.getId())</t>
-  </si>
-  <si>
-    <t xml:space="preserve">$flag: FlaggedPatient(patientId == $patient.getId(), message == $param)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insert(new FlaggedPatient($patient.getId(), $param));</t>
+    <t xml:space="preserve">not PatientFlag(patient == $patient)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$flag: PatientFlag(patient == $patient, message == $param)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insert(new PatientFlag($patient, null, $param));</t>
   </si>
   <si>
     <t xml:space="preserve">modify($flag){ setMessage($param) }</t>
@@ -502,8 +502,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>